<commit_message>
Changes to be committed:    (use "git reset HEAD <file>..." to unstage)
	modified:   trunk/MoveGenerator/Map_pins.xlsx
</commit_message>
<xml_diff>
--- a/trunk/MoveGenerator/Map_pins.xlsx
+++ b/trunk/MoveGenerator/Map_pins.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
@@ -192,8 +192,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,6 +313,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -347,6 +348,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -522,14 +524,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
@@ -540,7 +542,7 @@
     <col min="9" max="9" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -572,7 +574,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="2:11">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -600,8 +602,11 @@
       <c r="J3">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="2:11">
+      <c r="K3">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -629,8 +634,11 @@
       <c r="J4">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="2:11">
+      <c r="K4">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -658,8 +666,11 @@
       <c r="J5">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="2:11">
+      <c r="K5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -687,8 +698,11 @@
       <c r="J6">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="2:11">
+      <c r="K6">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -716,8 +730,11 @@
       <c r="J7">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="2:11">
+      <c r="K7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -745,8 +762,11 @@
       <c r="J8">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="2:11">
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -774,8 +794,11 @@
       <c r="J9">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="2:11">
+      <c r="K9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>11</v>
       </c>
@@ -803,8 +826,11 @@
       <c r="J10">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="2:11">
+      <c r="K10">
+        <v>-44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>12</v>
       </c>
@@ -832,8 +858,11 @@
       <c r="J11">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="2:11">
+      <c r="K11">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>13</v>
       </c>
@@ -861,8 +890,11 @@
       <c r="J12">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="2:11">
+      <c r="K12">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>14</v>
       </c>
@@ -890,8 +922,11 @@
       <c r="J13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="2:11">
+      <c r="K13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>15</v>
       </c>
@@ -919,8 +954,11 @@
       <c r="J14">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="2:11">
+      <c r="K14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>16</v>
       </c>
@@ -946,10 +984,13 @@
         <v>36</v>
       </c>
       <c r="J15">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11">
+        <v>26</v>
+      </c>
+      <c r="K15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>17</v>
       </c>
@@ -977,8 +1018,11 @@
       <c r="J16">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="2:10">
+      <c r="K16">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>18</v>
       </c>
@@ -1006,8 +1050,11 @@
       <c r="J17">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="2:10">
+      <c r="K17">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>19</v>
       </c>
@@ -1035,8 +1082,11 @@
       <c r="J18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="2:10">
+      <c r="K18">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>20</v>
       </c>
@@ -1064,8 +1114,11 @@
       <c r="J19">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="2:10">
+      <c r="K19">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>21</v>
       </c>
@@ -1093,8 +1146,11 @@
       <c r="J20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="2:10">
+      <c r="K20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>22</v>
       </c>
@@ -1122,8 +1178,11 @@
       <c r="J21">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="2:10">
+      <c r="K21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>23</v>
       </c>
@@ -1151,8 +1210,11 @@
       <c r="J22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="2:10">
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>24</v>
       </c>
@@ -1180,8 +1242,11 @@
       <c r="J23">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="2:10">
+      <c r="K23">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>25</v>
       </c>
@@ -1209,8 +1274,11 @@
       <c r="J24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="2:10">
+      <c r="K24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>48</v>
       </c>
@@ -1224,7 +1292,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="2:10">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>48</v>
       </c>
@@ -1245,12 +1313,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -1258,12 +1326,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>